<commit_message>
enhance AI for extracting receiveDate, refNo and sender
</commit_message>
<xml_diff>
--- a/preprocess/document_data.xlsx
+++ b/preprocess/document_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nitieii/Documents/TECHTACK/MRB Project/Source Code/AI-Document-Classifier/preprocess/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{D78A449D-20A3-C640-8F37-068CAC31A368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF6C7A91-AF62-7643-91FB-EE731AF410F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16800" yWindow="500" windowWidth="16800" windowHeight="20500" xr2:uid="{AB76A99D-4172-D045-871A-E199E7B93049}"/>
+    <workbookView xWindow="19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{AB76A99D-4172-D045-871A-E199E7B93049}"/>
   </bookViews>
   <sheets>
     <sheet name="document_data" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="93">
   <si>
     <t>title</t>
   </si>
@@ -1135,6 +1135,1008 @@
 ALSTOM Transport S.A. ~ HANOI LINE 3/ CP06 Project Office , 77
 Suite 902, Capital Tower, 109 Tran Hung Dao Street, Cua Nam Ward, Hoan Kiem District, Hanoi, Vietnam
 Tel: + 84 ow 3956 4999 — Fax: +84 (0)24 3967 4999
+</t>
+  </si>
+  <si>
+    <t>Agreement for consultant services made on the 2nd January 2016</t>
+  </si>
+  <si>
+    <t>Cc
+Spettle
+Hyundai - Ghella .J.V.
+18th Floor, VIT Tower
+519 Kim Ma Street
+Bah Dish District
+Hanoi - Vietnam
+Tax Code: 0107123332
+Fattura n°2017/348 del 20/12/2017
+(invoice n°2017/348 dated 12/20/2017)
+Oggetto: Contratto di servizi del 2 Gennaro 2016 per consulenza di personale e tecnico specializzati
+(Object: Agreement for consultant services made on the 2nd January 2016)
+- Attivita di consulenza da Ottobre a Dicembre 2017 delle seguenti figure:
+(-Consultant Service from October to December 2017)
+Nome . Posizione |. Periods | Imports mersie| Totals
+(Name) (Position) | Period Monthly fee Total Amount
+Braulio Bautista | Deputy Project Manager | Ott.- Dec. 2017 | $ 24.533,00 | $ 73.599,00
+Bells Tiziano | Deputy Administrative Manager Ott.- Dec. 2017 | $ 23.633,00 | $ 70.899,00
+Mai Van That Ugen | Arch. Engineer | Ott.- Dec. 2017 | $ 13.717,00 | $ 41.151,00
+Totals fattura $ 185.649,00
+(Total invoiced)
+Non imponibile iva art.7 ter del DPR n.633/72 e successive modificazioni.
+(VAT invoice is not taxable pursuant to art. 7ter, Presidential Decree 633/72)
+Pagamento: 60 gg data ricezione fattura
+(terms of payment: whitin 60 days after receipt of the invoice)
+Bank transfer details: Monte dei Paschi di Siena
+Rome - Italy
+IBAN: In33 H 01030 03233 000000003829
+SWIFT: PASCITMMROM
+Gh px
+Ư Seer Ghella S.p.A. 00195 Roma (Italia) - Via Pietro Borsieri, 2/A - Cap. Soc. € 60.000.000,00 int vers
+ch Tel. +39 06 45603.1 - Fax +39 06 45603040 - Part IVA 00898971007 - R.E.A. 330024
+ae Registry Impress di Torna e Cod Fiscate 00462220583
+e-mail: roma@ghella.com - PEC: ghellaspa@pec.it - www.ghella.com</t>
+  </si>
+  <si>
+    <t>Pursuant to the agreement for consultant service of 1% Jan. 2016 by Hyundai E&amp;C-
+Ghella Joint Venture and Hyundai Engineering &amp; Construction Co., Ltd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyundai Blog., 75 Yolgok-ro,
+A HYUNDAI Jongno-gu, Seoul, Korea
+ENGINEERING &amp; CONSTRUCTION
+T 82 2 746 3598 F 82 2 746 3920
+INV, Ns : IEOE-1712-0085 31. Dec, 2017
+To : Lt HYUNDAI E&amp;C-GHELLA-To GOI THAU Co-03 De TUYỂN DUONG SAT De THI
+DIEM To He, DOAN NHON-Gt He
+ATTN : Mr, Kim Do Gyoon / Project Manager
+Re : Request for Payment
+INVOICE
+Pursuant to the agreement for consultant service of 1% Jan. 2016 by Hyundai E&amp;C-
+Ghella Joint Venture and Hyundai Engineering &amp; Construction Co., Ltd.
+C We would like to request payment for the Fee as follows ;
+@ AMOUNT DUE
+Fee (4' qtr. 2017 Year) Up 731,487
+Total Amount U$ 731,487
+® ACCOUNT INFORMATION
+_ CNRENS BETAS
+. Beneficiary HYUNDAI ENGINEERING &amp; CONSTRUCTION Co., LTD
+. Bank KOREA EXCHANGE BANK (KiB)
+. Swift Code KOEXBHBM
+——-
+= „ Account Number 5202000067
+5To FLOOR YATEEM CENTER BLDG P.O.BOX 5767,
+MANAMA, BAHRAIN
+. Address
+% NOTE
+1, Payment can be made by telegraphic transfer to Hyundai Engineering &amp; Construction
+Co., Ltd’s A/C as amore-mentioned.
+2. Lt HYUNDAI E&amp;C-GHELLA-To GOI THAU Co-03 De TUYEN DUONG SAT De THI DIEM To
+He, DOAN NHON-Gt He has a responsibility to bear any kind of tax arisen from this
+payment of expenses.
+HYUNDAI ENGINEERING &amp; CONSTRUCTION Co., LTD
+Soo Hyun
+Soo Hyun J&amp;ng
+</t>
+  </si>
+  <si>
+    <t>X4440o00112 —
+4l Ghella
+Spent le
+Hyundai - Ghella J.V.
+18th Floor, VIT Tower
+519 Kim Ma Street
+Bah Dish District
+Hanoi - Vietnam
+Tax Code: 0107123332
+Fattura n°2018/103 del 30/03/2018
+(invoice n°2018/103 dated 03/30/2018)
+of Oggetto: Contratto di servizi del 2 Gennaro 2016 per consulenza di personale e tecnico specializzati
+(Object: Agreement for consultant services made on the 2nd January 2016)
+- Attivita di consulenza da Gennaro a Marzo 2018 delle seguenti figure:
+@ Consyftent Service from January to March 2018)
+Nome Posizione l | “Periods ¡ Imports tensile Totals ~
+i_____ (Name) — (Position) Period __ | Monthly fee Total Amount _
+Braulio GEMIEE | Deputy So MEETS [Sen- Mar. 2018| $ 24.533,00 |$ 73.599,00
+Bells Tiziano [pe SBMb Administrative MEH Gen.- Mar. 2018 j 23.633,00 | $ 70.899,00
+L_———.-. re —= — —
+Mai Van Use Gen - re Arch. Engineer [Sam Mar. ais, s 13.717,00 |$ 41.151,00
+Totals fattura $ 185.649,00
+{Total invoiced)
+Non imponibile iva art.7 ter del DPR n.633/72 e successive modificazioni.
+{ (VAT invoice is not taxable pursuant to art. 7ter, Presidential Decree 633/72)
+Pagamento: 60 gg data ricezione fattura.
+(terms of payment: whitin 60 days after receipt of the invoice)
+Bank transfer details. Monte dei Paschi di Siena
+Rome - Italy
+IBAN: In33 H 01030 03233 000000003829
+SWIFT: PASCITMMROM
+The sp A.
+Ghella S.p.A. 00195 Torna (Italia) - Via Pietro Borsien, 2/A - Cap. Soc. € 60,000.000,00 int. vers
+So Tel. +39 06 45603.1 - Fax +39 06 45603040 - Part IVA 00898971007 - R.E.A, 330024
+ICIC Registry Impress di Roma e Cod. Fiscale 00462220583
+e-mail. roma@ghella.com - PFC: ghellaspa@pec it - www.ghella com
+b.
+7</t>
+  </si>
+  <si>
+    <t>Pursuant to the agreement for consultant service of 1* Jan. 2016 by Hyundai E&amp;C-
+Ghella Joint Venture and Hyundai Engineering &amp; Construction Co., Ltd.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyundai Blog., 75 Yolgok-ro,
+A HYUNDAI Jongno-gu, Seoul, Korea
+ENGINEERING B CONSTRUCTION
+T 82 2 746 3598 F 82 2 746 3920
+INV. Ns : IEOE-1803-0054 31. Mar. 2018
+To : Lt HYUNDAI E&amp;C-GHELLA-To GOI THAU Co-03 De TUYEN DUONG SAT De THI
+DIEM To He, DOAN NHON-Gt He
+ATTN : Mr. Kim Do Gyoon / Project Manager
+Re : Request for Payment
+INVOICE
+Pursuant to the agreement for consultant service of 1* Jan. 2016 by Hyundai E&amp;C-
+Ghella Joint Venture and Hyundai Engineering &amp; Construction Co., Ltd.
+ft We would like to request payment for the Fee as follows ;
+@ AMOUNT DUE
+3. Swift Code KOEXBHBM
+4. Account Number 5202000067
+STH FLOOR YATEEM CENTER BLDG P.O.BOX 5767,
+5. Address
+MANAMA, BAHRAIN
+* NOTE
+1. Payment can be made by telegraphic transfer to Hyundai Engineering &amp; Construction
+Co., Ltd's A/C as amore-mentioned.
+2. Lt HYUNDAI E&amp;C-GHELLA-To GOI THAU Co-03 De TUYỂN DUONG SAT De THI DIEM To
+He, DOAN NHON-Gt He has a responsibility to bear any kind of tax arisen from this
+payment of expenses.
+Seo 7722 —
+Soo Hyun Jung
+Representative Director
+So
+</t>
+  </si>
+  <si>
+    <t>Consultant Service rendered by Monitoring Manager from July to September 2021 as per agreement dated 2 January. 2020</t>
+  </si>
+  <si>
+    <t>Spent.le
+Hyundai E&amp;C - Ghella J.V.
+NgocKhanh parking Area.
+Kim Ma Street
+Ba Dish District
+Hanoi - Vietnam
+Tax Code: 0107123332
+Fattura n° Re21000063 de! 30/09/2021
+(invoice n Re21000063 dated 30 September, 2021)
+Servữio di consulenza rest dai responsabile del monitoraggio del progetto nal periods luglio - settembre 2021, come da
+contratto del 02/01/2020.
+(Consultant Service rendered by Monitoring Manager from July to September 2021 as per agreement dated 2 January. 2020)
+Nome | Posizione Ï Periods | Total months | imports 1 mensiie | ““Totals
+(Name) (Position) _| _ Period presence Monthly fee Total Amount
+Antonio Di Pinto | Monitoring Manager lug -set. 2oat| 3 [s 10.000.00 : $ 30.000,00 |
+=e - _ wee - ee oe we eee J
+Totals fattura $ 30.000,00
+{Total invoiced)
+Non imponibile va art.7 ter del OPR n.B33/72 @ successive modificazionI.
+(VAT invoice Is not taxable pursuant fo art. 7tar, Presidential Decree 633/72)
+Pagamento: 60 gg data ricezione fattura
+(terms of payment: whitin 60 days after receipt of the invoice)
+Bank transfer metals: Monte det Paschi di Siena
+Rome - Italy
+IBAN: In33 H 01030 03233 000000003829
+SWIFT: PASCITMMROM
+Ghella S.p.A.
+(tosictoa esbio
+ee
+4 ` Ghetia S px › Roma ita +a) - Via Veto Borsior, 2fa Cap. Soc © 00.090 009.00 int vers
+Re}A © Tel ~39 06 455031 - Fax +39 06 45603040 2ar: IVA 0089897100’ - REA 330024
+Registry impress di Rome e Cod Í sca.e 2402229983
+epee Of
+e mãi roma@ghellaccm - PEC grelasoa@sec.it way ghela com</t>
+  </si>
+  <si>
+    <t>Cp02 - Update the As-built documents</t>
+  </si>
+  <si>
+    <t>ĐOSCO POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+2°¢ Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+E&amp;C tel: 84-24-37957001 Fax: 84-24-37957005 Website: www,poscoenc.com
+Date - January AƠ* 2021
+Ref. No.: PSC-MLT-00004 -22-E
+To: Mr. David CHEVALLIER- Acting Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 -Hoa Bind Building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-3791 85 40 Fax: 84-24-37 91 85 44
+Ce: Mr. Nguyen Cao Mind - General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: CC2 Building, Dong Tau Urban Area, Hoang Mai, Hanoi
+Tel: 84-24-39 43 51 27 Tel: 84-24-39 43 51 26
+Subject: Co02 - Update the As-built documents
+Reference:
+[a] PSC-MLT-00266-21-E/V dated on 02/11/2021,
+Dear Sir,
+Refer to letter [a] and the actual construction at site, the Contractor would like to submit the updated as-built
+documents attached herewith.
+Your understanding and support would be highly appreciated.
+Se ee
+Of CHUL Km
+Project Manager
+Attachment: Co02 - List of As-built documents
+1</t>
+  </si>
+  <si>
+    <t>Submission of Construction Photographs [November, 2022]</t>
+  </si>
+  <si>
+    <t>ĐOSCO POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+Date -
+Ref, No.:
+To:
+Subject:
+Dear Sir,
+2™ Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+E&amp;C Tel: 84-24-37957001 Fax: 84-24-37957005 Website: www,0oscoenc.com
+January 10, 2023
+PSC-MLT-00005-23-E
+Mr. Alain BECHEREAU - Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 -Hoa Bind Building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-3791 85 40 Fax: 84-24-37 91 85 44
+Mr. Nguyen Cao Mind — General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: CC2 Building, Dong Tau Urban Area, Hoang Mai, Hanoi
+Tel: 84-24-39 43 S1 27 Tel: 84-24-39 43 51 26
+Co02 — Submission of Construction Photographs [November, 2022]
+We would like to express our thankful mind to your cooperation and support during our work
+implementation so far.
+Referring to Sub-clause 1.10 Photographs, Part In — Chapter Il-2 Technical requirements, we would like to
+submit the Construction Photograph showing the construction activities in November 2022 as enclosed
+herewith.
+ebook forward to your kind support and further cooperation.
+Attachment:  - Construction photographs
+-1 DVD
+HAI</t>
+  </si>
+  <si>
+    <t>Co02-— Submission of Performance Security</t>
+  </si>
+  <si>
+    <t>DOSC POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+2°*Floor, My Dish Plaza, No.138 Tran Bind Str., Nam TuLiem District, Hanoi, Vietnam
+E&amp;C Tel: 84-24-37957001 Fax: 84-24-37957005 Website: www.pOscoenc.com
+Date: January Ant 2022
+Ref. No.: PSC-MLT-00006 -22-E
+To: Mr. Nguyen Cao Mind — General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: Building CC-2, Dong Tau New Urban Zone, Hoang Mai District, Hanoi
+Tel: 84-24-39 43 5] 27 Fax: 84-24-39 43 51 26
+Ce: Mr. David CHEVALLIER - Acting Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 -Hoa Bind building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-37 91 85 40 Fax: 84-24-37 91 85 44
+Subject:  Co02-— Submission of Performance Security
+Dear Sir,
+With reference to:
+1. PIC-MLT-05843-21-E/V “Co02 ~ Validity of Performance Security &amp; Advance Payment Security”
+dated on December 15, 2021;
+Pursuant to Clause 4.2 GCC [Performance Security], the Contractor would like to submit the notarize
+document of Performance Security as follows:
+Guarantee No. Amendment No. Cop y of
+Original
+0441GAs130800002
+Notarized
+Translation
+Document
+Performance Security
+01 set
+| 0441GADI30800003 |
+The original copy of Performance Security is attached herewith.
+Your cooperation would be highly appreciated.
+Attachment: 1. Performance Security (1 copy of original in English; 1 notarized translation in
+Vietnamese)</t>
+  </si>
+  <si>
+    <t>Submission of Construction Photographs [December, 2022]</t>
+  </si>
+  <si>
+    <t>OOSCO POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+Date:
+Ref, No.:
+To:
+Subject:
+Dear Sir,
+24 Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+E&amp;C tel: 84-24-37957001 Fax: 84-24-37957005 Website: www.poscoenc.com
+January 11, 2023
+PSC-MLT-00006-23-E
+Mr. Alain BECHEREAU - Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 —Hoa Bind Building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-3791 85 40 Fax: 84-24-37 91 85 44
+Mr. Nguyen Cao Mind — General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: CC2 Building, Dong Tau Urban Area, Hoang Mai, Hanoi
+Tel: 84-24-39 43 51 27 Tel: 84-24-39 43 51 26
+Co02 — Submission of Construction Photographs [December, 2022]
+We would like to express our thankful mind to your cooperation and support during our work
+implementation so far.
+Referring to Sub-clause 1.10 Photographs, Part In - Chapter In-2 Technical requirements, we would like to
+submit the Construction Photograph showing the construction activities in December 2022 as enclosed
+herewith.
+We look forward to your kind support and further cooperation.
+Lt
+SORE Km
+Project Manager
+Attachment:  - Construction photographs
+-1 DVD
+11</t>
+  </si>
+  <si>
+    <t>Reply to the letter Co07 Notice on delay of cable connection and integrated system
+T&amp;C schedule</t>
+  </si>
+  <si>
+    <t>OOSCO POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+Date :
+Ref. No.:
+To:
+Subject:
+Dear Sir,
+2°° Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+E&amp;C Tei: 84-24 3795 7001 Fax: 84 24-3795 7005 Website: www.poscoenc.com
+January 26”, 2022
+PSC-MLT-00044 -22-E
+Mr. Michel INTROVIGNE - Project Manager
+Project Office HPLML/Co07
+Address: 06th floor, Toserco building, 273 Kim Ma, Giant Vo Ward, Ba Dish Dist., Hanoi
+Tel: 84-24-3245 4117
+Mr. Nguyen Cao Mind - General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: Building CC-2, Dong Tau New Urban Zone, Hoang Mai District, Hanoi
+Tel: 84-24-39 43 51 27 Tel: 84-24-39 43 51 27
+Mr. David CHEVALLIER -Acting Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 -Hoa Bind building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-37 9] 85 40 Fax: 84-24-37 91 85 44
+Co02 - Reply to the letter Co07 Notice on delay of cable connection and integrated system
+T&amp;C schedule
+Reference:
+a. CSR-MLT-00243-21-E-V received date 18/11/2021
+PSC-MLT-00272-21-E dated 04/11/2021
+PSC-MLT-00209-21-E dated 23/08/2021
+PSC-MLT-00304-21-E dated 31/12/2021
+CSR-MLT-00013-22-E-V received date 20/01/2022
+pane
+As we have mentioned on the letter [d], we have spent our effort for the cable connection, but not fully
+success as here under table:
+L~
+| soi, S02 S03 S04 | sos | S06 S07 S08
+Equip.
+to Tm te
+FAS power Of (*) | Of (*) Of (*) | Of (*) | Of(*)| Of (*) Of (*) Of (*)
+= | _—— — | —] ——
+FFS (pump Done Done0] ¡ Done 01 Done | Done Don Done Done 01
+room) 28/2/2022 | 28/2/2022 ° 28/2/2022
+Before
+. e
+Outdoor ELE Done Done Done Done none | Done 28/2/2022 Done
+Outdoor ESC Done Done rosie Done | Done Crop (Of Done tone
+I 28/2/2022 28/2/2022 28/2/2022
+For the FAS power Of, we would like to highlight that the FAS power source, which goes through DB-
+En and UPS, has been connected, tested and ready for Power Of. Only an issue is that the power Of the
+UPS will start the equipment warranty period. But PSC’s equipment does not request any power from this
+equipment. Therefore, we would like to request your payment confirmation for the warranty cost of the
+Co02 UPS equipment before power Of to your equipment.
+By this letter, we would like to update the connection schedule of remaining cable (before 28/02/2022)
+and this activity will be coordinated with your team for termination for the outdoor equipment as your
+requirement.
+1⁄2</t>
+  </si>
+  <si>
+    <t>Gap analysis report on new Regulations and standards for firefighting</t>
+  </si>
+  <si>
+    <t>OOSCO POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+2” Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+E&amp;C Tel: 84-24-37957001 Fax: 84-24-37957005 Website: www.poscoenc.com
+Date : January 262022
+Ref. No.:  PSC-MLT-00042-22-E
+To: Mr. David CHEVALLIER -Acting Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 -Hoa Bind Building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-3791 85 40 Fax: 84-24-37 91 85 44
+Ce: Mr. Nguyen Cao Mind - General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: CC2 Building, Dong Tau Urban Area, Hoang Mai, Hanoi
+Tel: 84-24-39 43 51 27 Tel: 84-24-39 43 5] 27
+Subject:  Co02 - Gap analysis report on new Regulations and standards for firefighting
+Reference:
+fa] Engineer's letter PIC-MLT-05048-21 dated 21/10/2021 regarding Co02- Notice to the
+Contractor failure to comply with applicable law and regulation of firefighting
+[b] Engineer's lever PIC-MLT-03455-21 dated 07/07/2021 regarding Co00- Engineers
+Instruction - New Regulations and standards for firefighting
+Íc]} Engineer's letter PIC-MLT-04601-2] dated 27/09/2021 regarding Co00- Request for
+analysis depot on new Regulations and standards for fire fighting
+{d] PSC letter No. PSC-MLT-00268-21-E dated 02/11/2021 regarding new regulation &amp;
+standard for firefighting
+fe] PSC letter No. PSC-MLT-00289-21-E - dated 03/12/2021 regarding Gap analysis report on
+new Regulation &amp; standards for FF - fire resistance categories &amp; fire hazard classification
+of elevated station
+{f] PIC-MLT-05859-21-E- dated 16/12/2021 regarding gap analysis report on the updated
+QCVN regulation (fire, life &amp; safety)
+Dear Sir,
+Together with letter [d] and [e], PSC would like to submit the Gap analysis report on new Regulations and
+standards for firefighting as the attachment.
+As the result of impact assessment on the new standards and regulations on civil works, there is no change
+of the station and rooms which has been built as the To design and approval from Ft for firefighting and
+fire prevention.
+We would like to highlight that this is the assessment result which base on a construction contractor's
+experience and study only under his obligation in the Conditions of the Contract.
+Your consideration and coordination in this regard are highly appreciated.
+Project Manager
+Attachment: Co02- Gap Analysis summary between new &amp; current applying standards and regulations — 01 page
+1⁄1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ooec
+E&amp;C Tel: 84-24-3795 7001
+Fax: 84-24-3795 7005
+Mr. Michel INTROVIGNE - Project Manager
+O POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+2°? Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+Website: www.poscoenc.com
+Address: 06th floor, Toserco building, 273 Kim Ma, Giant Vo Ward, Ba Dish Dist., Hanoi
+Mr. Nguyen Cao Mind - General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: Building CC-2, Dong Tau New Urban Zone, Hoang Mai District, Hanoi
+Tel: 84-24-39 43 51 27
+Mr. David CHEVALLIER -Acting Project Director
+Address: Level 12 -Hoa Bind building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Fax: 84-24-37 91 85 44
+Co02 - Response to the letter Co07 Construction &amp; T&amp;C interface tracker
+CSR-MLT-00216-21-E-V received date 26/10/2021
+b. PSC-MLT-306-21-E-V dated 31/12/2021
+CSR-MLT-00011-22-E received date 14/01/2022
+Date : January 27, 2022
+Ref. No.: PSC-MLT-00013-22-E
+To:
+Project Office HPLML/Co07
+Tel: 84-24-3245 4117
+Ce:
+Tel: 84-24-39 43 51 27
+Ce:
+Systra Hanoi Metro Project Office
+Tel: 84-24-37 91 85 40
+Subject:
+Reference:
+a.
+c.
+Dear Sir,
+Together with the letter [b], we would like to reply for the letter [c} as it related item as following:
+a a a |
+Sq. Area/item Clarification/Request Remarks
+1 Water at HVAC |- Co07’s responsibility to control the condensate water to drop in
+rooms to floor drain, and we will monitor this issue when your ECS
+system is under operation.
+- For the epoxy and floor finishing work, this issue will be
+finalized between Co02 and PIC as the acceptance of work
+procedure.
+2 Water at public|- The additional roof at the escalator/stair openings (04 areas) has
+area been completed already. Once again, we would like to inform|
+that the Co02’s Finishing items are completed as the approved
+CDD.
+- Expansion joint is constructed as per approved Construction
+Design drawing and Material approved. Water leakage in public
+area is not Co02’s responsibility.
+- Indoor ELE: Drainage pipe is installed
+- Drainage of intermediate ESC: original not Co02’s scope of
+work.
+|- The additional works schedule: will be provided until finalize
+the Vs issue with PIC/MRB
+1
+3 Pumping - Neither Co02 nor Co07 can refuse the responsibility to protect
+system for|his equipment under construction period as the contract under
+‘outdoor actual site condition.
+ELE/ESC
+1/2
+</t>
+  </si>
+  <si>
+    <t>Response to the letter CP07 Construction &amp; T&amp;C interface tracker</t>
+  </si>
+  <si>
+    <t>Draft Contract Amendment No. 10 [Temporary Extension of Time for Completion
+from 31/12/2021 to 31/12/2022 (EOT3); Clarifying Mon dated 03/06/2013 regarding
+Financial Negotiation of Profit, other Direct Cost, Overhead; Supplement 01 Variation
+request; Update Contract Price]</t>
+  </si>
+  <si>
+    <t>ĐOSCO POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+2™ Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+E&amp;C tel: 84-24-37957001 Fax: 84-24-37957005 Website: www.poscoenc.com
+Date: February 11, 2022
+Ref. No.: PSC-MLT-0004b-22-E
+To: Mr. David CHEVALLIER -Acting Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 -Hoa Bind building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-62 58 30 40 Fax: 84-24-37 91 85 44
+Ce: Mr. Nguyen Cao Mind - General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: Building CC-2, Dong Tau New Urban Zone, Hoang Mai District, Hanoi
+Tel: 84-24-39 43 51 27 Fax: 84-24-39 43 51 26
+Subject: Co02 - Draft Contract Amendment No. 10 [Temporary Extension of Time for Completion
+from 31/12/2021 to 31/12/2022 (EOT3); Clarifying Mon dated 03/06/2013 regarding
+Financial Negotiation of Profit, other Direct Cost, Overhead; Supplement 01 Variation
+request; Update Contract Price]
+Dear Sir,
+In reference with:
+e Correspondence among MRB/PIC/PSC via email;
+After reaching the agreement with the Employer and the Engineer regarding the above-mentioned content,
+the Contractor would like to hereby submit the Draft Contract Amendment no. 10 for Temporary
+Extension of Time for Completion from 31/12/2021 to 31/12/2022 (EOT3); Clarifying Mon dated
+03/06/2013 regarding Financial Negotiation of Profit, other Direct Cost, Overhead; Supplement 01
+Variation request; Update Contract Price] for your review.
+We look forward to your consideration in order to facilitate the contract implementation.
+Draft Contract Amendment No. 10 [Temporary Extension of Time for Completion
+from 31/12/2021 to 31/12/2022 (EOT3); Clarifying Mon dated 03/06/2013
+regarding Financial Negotiation of Profit, other Direct Cost, Overhead;
+Supplement 01 Variation request; Update Contract Price]
+2. Minutes of Negotiation (Mon) for Contract Amendment No. 10 regarding Time
+Extension; Clarifying Mon dated 03/06/2013 Regarding Financial Negotiation of
+Profit, other Direct Cost, Overhead; Supplement 01 Variation Request (Vs)</t>
+  </si>
+  <si>
+    <t>Request for agreement in principle for Vs of Additional lighting works for storage rooms
+under staircase at concourse level and for areas of outdoor elevator control cabinets in elevated
+stations</t>
+  </si>
+  <si>
+    <t>ĐOSCO POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+2“£ Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+E&amp;C tel: 84-24-37957001 Fax: 84-24-37957005 Webste: www.poscoenc.com
+Date: March 2, 2022
+Ref No: PSC-MLT-00024-22-E
+To: Ông David CHEVALLIER - Acting Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 -Hoa Bind Building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-3791 85 40 Fax: 84-24-37 91 85 44
+Ce: Mr. Nguyen Cao Mind - General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: CC2 Building, Dong Tau Urban Area, Hoang Mai, Hanoi
+Tel: 84-24-39 43 5] 27 Tel: 84-24-39 43 51 26
+Subject: Co02—- Request for agreement in principle for Vs of Additional lighting works for storage rooms
+under staircase at concourse level and for areas of outdoor elevator control cabinets in elevated
+stations
+Ref : [a] PIC-MLT-04773-21-E, dated 06/10/2021
+[b] 1797/DSDT-De 1, dated 05/10/2021
+Dear Sir,
+As per your request [a], the Contractor would like to issue this specific letter requesting agreement in
+principle for Vs of “Additional lighting works for storage rooms under staircase at concourse level and
+for areas of outdoor elevator control cabinets in elevated stations”.
+Based on the site situation and the Engineer’s instruction, the Contractor has developed the drawing of
+Additional lighting works for storage rooms under staircase and for areas of outdoor elevator control
+cabinets in elevated stations (ref: Co2-Co-22-0075-A) which is being reviewed by PIC; therefore, the
+Contractor would like to propose MRB/PIC to consider to approve in principle for this Vs.
+The detail of variation and the draft summary table of estimated additional items can be found in the
+attachment #1. The Contractor will reflect the detailed calculation and basis in the Variation report later,
+after getting the agreement in principle from the Employer and Engineer.
+Your consideration and cooperation would be highly appreciated.
+Of CHUL Km
+Project Manager
+Attachment 1: 1. Preliminary cost estimate for additional lighting works for storage rooms ---- 02 pages
+under staircase and for areas of outdoor elevator control cabinets in
+elevated stations
+1⁄1</t>
+  </si>
+  <si>
+    <t>Submission of Construction Photographs [January, 2022]</t>
+  </si>
+  <si>
+    <t>ĐOSCO POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+2 Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+E&amp;C tel: 84-24-37957001 Fax: 84-24-37957005 Website: www.poscoenc.com
+Date:  March of*2022
+Ref, No: PSC-MLT-00028-22-E
+To: Mr. David CHEVALLIER -Acting Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 -Hoa Bind Building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-3791 85 40 Fax: 84-24-37 91 85 44
+Ce: Mr. Nguyen Cao Mind — General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address; CC2 Building, Dong Tau Urban Area, Hoang Mai, Hanoi
+Tel: 84-24-39 43 51 27 Tel: 84-24-39 43 51 26
+Subject:  Co02— Submission of Construction Photographs [January, 2022]
+Dear Sir,
+We would like to express our thankful mind to your cooperation and support during our work
+implementation so far.
+Referring to Sub-clause 1.10 Photographs, Part In - Chapter In-2 Technical requirements, we would like to
+submit the Construction Photograph showing the construction activities in January 2022 as enclosed
+herewith.
+eee. forward to your kind support and further cooperation.
+Project Manager
+Attachment:  - Construction photographs
+-1 DVD
+1⁄1</t>
+  </si>
+  <si>
+    <t>Drainpipe for station 01 intermediate outdoor escalator</t>
+  </si>
+  <si>
+    <t>OOSCO POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+2 Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+E&amp;C Tel: 84-24-37957001 Fax: 84-24-37957005 Website: www,poscoenc.com
+Date: March 10%, 2022
+Ref, No..  PSC-MLT-00028-22-E
+To: Mr. David CHEVALLIER -Acting Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 -Hoa Bind Building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-3791 85 40 Fax: 84-24-37 91 85 44
+To: Mr. Nguyen Cao Mind - General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: CC2 Building, Dong Tau Urban Area, Hoang Mai, Hanoi
+Tel: 84-24-39 43 51 27 Tel: 84-24-39 43 51 26
+Subject: Co02- Drainpipe for station 01 intermediate outdoor escalator
+Ref: [a] PIC-MLT-00258-22-E dated 24/02/2022
+[b] PIC-MLT-02141-21-E dated 24/04/2021
+Dear Sir,
+Reference is made to your letter Ref. PIC-MLT-00258-22-E and we consider that there are some issues to be
+clarified by the Engineer as followings:
+As mentioned on the IRE No. Co07-IRE-Co02-008 dated 06/4/2021, Co02 Contractor is not in a position to
+deal with IFR document to finalize the technical agreement since there is neither scope of work assigned to
+Co02 related to the above subjected matter as quoted below from ICD 72-4.1 nor Co02’s contractual basis to
+make modification of Permanent Works without Engineer’s instruction in accordance with Sub-Clause 13.1
+of General Conditions of the Contract.
+1}: This equipment Is a special type of CPO7‘s escalator installed in the wir ạt the
+intermediate level (En1-S01), to there's no any structural px around the
+equipment.
+- This Item Is not included In the Co02's scope of work following the original
+contract and Box,
+In the matter of fact, different to below quoted PIC’s reminder from the aforementioned letter, we consider
+Instruction of the Engineer subject to Sub-Clause 3.3 of GCC hasn't been given and Co02 has no contractual
+basis to implement Permanent Works and complete works yet.
+We remind of Engineer's adjudication in letter [b] and require an updated status of the works and the
+forecast to complete the remaining installation and testing from Co02 Contractor.
+Therefore, in case Engineer pursues the above quoted adjudication you are kindly requested to issue an
+official instruction under Sub-Clause 3.3 of GCC for the Vs submission of this work item.
+Project Manager
+1⁄1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Station 6 En4 cladding — Clarification of changing aluminum to aluminum</t>
+  </si>
+  <si>
+    <t>DPOSC POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+24 Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+E&amp; Tel: 84-4-37957001 Fax: 84-4-37957005 Website: www .poscoenc.com
+Date : March 25, 2022
+Ref. No.: PSC-MLT-00089-22-E
+To:
+Ce:
+Mr. Nguyen Cao Mind - General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: Building CC-2, Dong Tau New Urban Zone, Hoang Mai District, Hanoi
+Tel: 84-24-39 43 51 27 Tel: 84-24-39 43 51 27
+Mr. David CHEVALLIER - Acting Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 ~Hoa Bind building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-37 91 85 40 Tel: 84-24-37 91 85 40
+Subject: Co02~ Station 6 En4 cladding — Clarification of changing aluminum to aluminum
+composite (respond to the Employer letter Ref.374/DSDT-Del)
+Reference:
+[a] 374/DSDT-De 1 dated 21/03/2022;
+[b] PIC-MLT-005 19-22 dated 24/02/2022;
+[c] PSC-MLT-00294-21 dated 17/12/2021;
+[d] PIC-MLT-05591-21 dated 24/11/2021;
+[e] PSC-IMP-TRE-WSE-S00-00394-B-4A;
+Dear Sir,
+The Contractor is in receipt of the Employer’s letter referenced [a] as mentioned above whereby the Employer
+requests to clarify the reason for changing aluminum to aluminum composite, the Contractor would like to
+respond as follows;
+1.
+In terms of technical aspects: According to the technical design drawings describing the En4 cladding
+part of station 6 is aluminum plate; however, this item is not included in the project's technical
+requirements and has not been applied for any item before. Therefore, according to project’s requirement,
+to be put into use, this aluminum cladding material will have to take steps including proposal of the
+applicable standard and then submission of the material source for approval. This approval process will
+take about 3 months. And the minimum time for importing materials is 03 months as the usual regulations.
+According to the agreed progress among parties, the arising items of the Co02 package will be completed
+before June 2022, including En4 Cladding — Station 6. Therefore, it is necessary to find another more
+suitable material approved for the same item to ensure the project progress. Referring to document ref.
+[e], the Contractor assessed that the aluminum composite plate used for the main roof of the station and
+also approved for the ticketing &amp; passenger information room met the criteria for technical aspects as
+well as the progress of the project. It is for this reason that the Contractor would like to change the
+aluminum plate to aluminum composite plate. This proposal has also been approved by the Engineer by
+letter ref. [d];
+1/2</t>
+  </si>
+  <si>
+    <t>The Contractor’s explanation on replacement of grass planting by concrete paving
+block in the median curb under the station</t>
+  </si>
+  <si>
+    <t>OOSCO POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+2 Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+E&amp;C Tel; 84-24-3795 7001 Fax: 84-24-3795 7005 Website: www.poscoenc.com
+Date: March 31°, 2022
+Ref. No.: PSC-MLT-00042 22-E
+To: Mr. Nguyen Cao Mind - General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: Building CC-2, Dong Tau New Urban Zone, Hoang Mai District, Hanoi
+Tel: 84-24-39 43 51 27 Tel: 84-24-39 43 $1 27
+To: Mr. David CHEVALLIER -Acting Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 -Hoa Bind building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-37 91 85 40 Fax: 84-24-37 91 85 44
+Subject:  Co02 — The Contractor’s explanation on replacement of grass planting by concrete paving
+block in the median curb under the station
+Dear Sir,
+Regarding the work item of Landscaping, planting grass (Oplismenus composites) in the median curb.
+Despite previous discussions during the preparation of the design documents for this item; however, the
+Contractor was recommended to respect the technical design with grass planting at the median curb under
+the station.
+However, according to the Contractor's experience. for the biological properties of oplismenus composites,
+it is very difficult for grass to grow well in the low light environment under the station, especially, the
+elevated stations are located close to residential areas, it is impossible for natural light to reach this area
+(please see the illustration at station S01 below).
+Lighting pattern at 10.0 As Lighting pattern at 3.0 Px
+Taking care of plants in an environment that lacks natural light like the median curb under the station will
+cause difficulties for the Operation Company (HMC) and incur additional costs;
+Therefore, PSC still maintained his proposal by replacing the grass planting by concrete paving block in
+the median area under the station. This proposal does not affect the quality or function of the station, but
+also optimized the design for this item, ensures environmental sanitation and be convenient for
+1+</t>
+  </si>
+  <si>
+    <t>Request for Provision of Assumed Access Date</t>
+  </si>
+  <si>
+    <t>AHYUNDA! HYUNDAI E&amp;C - GHELLA Ja
+4'hell Ngoc Khans Parking Area, Kim Ma Street, Ngoc Khans Ward, Ba Dish District, Hanoi, Vietnam
+Tel: +84 24 3237 3461 Fax: +84 24 3237 3462 Website: en.hdec.kr / www.ghella.com
+Date : 14/06/2021
+Ref. No.:  HGU-MLT-00437-21-E
+To: Mr. Nguyen Cao Mind — General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: CC2 Dong Tau Urban Area, Think List, Hoang Mai, Hanoi
+Tel: 84-24-3943 5127 Fax: 84-24-3943 5126
+To: Mr. Philippe BLANCHO - Project Director
+Systra Hanoi Metro Project Office
+Address: 12 floor - Hoa Bind Blog., 106 Hoang Quot Viet Str., Can Gray Dist., Hanoi
+Tel: 84-24-3791 8540 Fax: 84-24-3791 8544
+Subject: | Co03 - Request for Provision of Assumed Access Date
+Dear Sir,
+Ref. (i) Progress Meeting on 3 June 2021
+(ii) Employer letter ref. 194/DSDT-DAI dated 19 February 2021 (received on 22 Feb.
+2021)
+(iii) Engineer letter ref. PIC-00315-21-E dated 19 January 2021
+(v) _ Contractor letter ref. HGU-MLT-00027-21-E dated 12 January 2021 (Submission of
+Option 1 — Programme rev. 4A)
+As the Employer is well aware, the Assumed Access Date! of 22 December 2020 in the approved
+programme ref. (iv) has not been achieved as of the date of this letter and new Assumed Access Date
+shall be provided in order for the Contractor to plan the Works and update the current approved
+programme as requested at the Progress Meeting on 3 June 2021.
+As it was confirmed by the Employer in various meetings that he will complete land clearance of all
+remaining Site by the end of July 2021, the Contractor will update the approved completion programme
+based on the assumption that all remaining Site will be provided to the Contractor by 31 July 2021. i.e.
+used Access Date to be 31 2021.
+Should the le Engineer or the Employer have any objection on the above assumption, please let the
+He 03 DỰ
+rat ĐƯỜNs SAT | -
+ĐỒ ToỊ ToÍ OIE
+HỖ HÀ NỘI
+For and on 1 behalf of
+HYUNDAI E&amp;C - GHELLA JOINT VENTURE
+! Assumed access date for the remaining Site which has not been provided to the Contractor
+1⁄1</t>
+  </si>
+  <si>
+    <t>AMENDMENT No. 01 To AGREEMENT FOR CONSULTANT SERVICES</t>
+  </si>
+  <si>
+    <t>“AMENDMENT No. 01 To AGREEMENT FOR CONSULTANT SERVICES ˆˆ ˆ
+This Amendment No. 01 (the “Amendment No. 01”) is made and entered into this 1” day of February,
+2020, by and between:
+Hyundai E&amp;C - Ghella Joint Venture, having its registered office in Ngoc Khans parking area, Kim Ma
+Street, Bah Dish District, Hanoi, Vietnam, duly represented by Mr. Song Sang Min, Project Manager of the
+Joint Venture (the “Contractor”); and
+GHELLA SPA, a company duly organized and existing under the laws of Republic of Italy, having its
+registered office at Via Pietro Borsieri 2/a, 00195 Rome, Italy, duly represented by Mr. Andrea Lombardi
+(the “Consultant”).
+In this Amendment No. 01, the Contractor and the Consultant hereinafter referred to individually as the
+“Party” and collectively as the “Parties”.
+WHEREAS
+A. On21 August 2015, the Parties entered into a joint venture agreement, in order to perform the Project,
+fixing the terms and conditions for the operation and management of the joint venture and define
+the respective rights, interests, duties, obligations and liabilities (the “Joint Venture Agreement”);
+B. On 2 January 2016, the Parties entered into an Agreement for Consultant Services (the “Agreement”).
+Through the execution of the Agreement, the Consultant undertakes to provide specialized Personnel
+to the Contractor as defined in the Appendix: Breakdown of Consultant Service Fee for a specified
+period of time, for the provision of the Services;
+C. The Parties now desire to enter into this Amendment No. 01 to amend, modify and supplement
+certain provisions of the Agreement.
+NOW, THEREFORE, the Parties in consideration of the foregoing and the mutual promises and
+undertakings contained herein, do hereby agree as follows:
+1. INTERPRETATION
+1.1 Unless otherwise defined herein, all capitalized terms used in this Amendment No. 01 shall have the
+same respective meanings assigned to such terms in the Agreement, and all terms in this Amendment
+No. 01 shall be interpreted in the same manner as the terms used in the Agreement.
+1.2 Except as specifically amended by this Amendment No.1, the terms and conditions of the Agreement
+shall remain unchanged and continue in full force and effect.</t>
+  </si>
+  <si>
+    <t>Submission of Revised Alternative Design for D-Wall and Top Slab for Stations</t>
+  </si>
+  <si>
+    <t>HYUNDAI HYUNDAI E&amp;C - GHELLA Ja
+aan an pessoas Tri
+18th Floor, VIT Tower, 519 Kim Ma Street, Ngoc Khans Ward, Ba Dish District, Hanoi, Vietnam
+a Ghella Tel: +84 4 3237 3461 Fax: +84 4 3237 3462 Website: en.hdec.kr / www.ghella.com
+Date : 14/11/2017
+Ref. No: HGU-MLT-00404-17-E
+To: Mr. Alain BECHEREAU - Project Director
+Systra Hanoi Metro Project Office
+Address: 12 floor — Hoa Bind Blog., 106 Hoang Quot Viet Str., Can Gray Dist., Hanoi, Viet
+Nam
+Tel: 84-4-3791 8540
+Fax: 84-4-3791 8544
+Ce: Mr. Nguyen Cao Mind — General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: CC2 Dong Tau Urban Area, Think List, Hoang Mai, Hanoi.
+Tel: 84-4-39 43 5127 Fax: 84-4-39 43 51 26
+Subject: Co03— Submission of Revised Alternative Design for D-Wall and Top Slab for Stations
+Dear Sits,
+With reference to our previous discussion and Engineer’s design review and subsequently to our meeting
+held on 11 November 2017 at MRB office in relation to our proposed alternative design for the above
+subject. ;
+We would like submit our “Revised Alternative Design for D-Wall and Top Slab” attached herein and in
+compliance with the discussions in our meeting and in accordance with our project specification, standards
+and regulations.
+In this regard, we respectfully request to the Engineer their immediate approval of the above subject to
+enable us to proceed with further works.
+We would like to thanks to the Engineer and Employer for their support and cooperation during the design
+working sessions.
+Kim Do Gyoon
+Project Manager (
+4
+For and on behalf of
+HYUNDAI E&amp;C - GHELLA JOINT VENTURE
+Attachment: Report on Alternative design for Stations (D-wall and Top slab)
+W/</t>
+  </si>
+  <si>
+    <t>Comments on TREE REPORT FOR IMPROVEMENT Of SMALL KIM MA
+STREET As STATION 9 FOR PERMIT APPLICATION</t>
+  </si>
+  <si>
+    <t>EECEIVED
+30 -1?- 2017
+HYUNDAI E &amp; C-GHELLA Ja
+AUBVAV TẾ De \P
+Q| TUYỂN ĐƯỜNs SẮT
+Date: 29/12/2017 Z\ OTIETPHN ByẠN
+Ref. No.:  PIC-MLT-04796-17-E
+To: Mr. Nguyen Cao Mind — General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: CC2 building, Dong Tau Urban Area, Hoang Mai, Hanoi
+Tel: 84-4-39 43 51 27 Fax: 84-4-39 43 51 26
+Ce: Mr. Kim Do Gyoon - Project Manager
+Hyundai E&amp;C - Ghella Ja
+Address: Floor 18 - VIT Tower - 519, Kim Ma str., Ngoc Khans, Hanoi
+Tel: 84-24 32 37 34 61 Fax: 84-24-32 37 34 62
+Subject: CPO3 - Comments on TREE REPORT FOR IMPROVEMENT Of SMALL KIM MA
+STREET As STATION 9 FOR PERMIT APPLICATION
+(HGU-IMP-TRE-WAO-L10-00018-B-1A}
+(Submission Ref: HGU-MTS-00582-17-B received on 20/12/2017)
+Dear Sir,
+In reply to the submitted document referenced above, PIC grants the status of SONO (Statement Of
+No Objection) as a basis for you to assess the contractor's documentation.
+If MRB has no additional comments on the above referenced document, we kindly recommend MRB
+9 instruct the contractor to submit to PIC 10 signed and stamped copies for final approval.
+BYSTRAS.A &gt;.
+THAU DVTV To By \”
+sin BECHEREAU
+Project Director
+—o-
+SYSTRA Hanoi Metro Project
+12th floor - Hoa Bind Building, 106 Hoang Quot Viet Str. » Can Gray Distr. s Ha Noi s Viet Nam
+Tel. +84-4 37918540 +» Fax +84437918544 + Website: www.systra.com</t>
+  </si>
+  <si>
+    <t>Notice on the readiness for acceptance of firefighting
+Reference:</t>
+  </si>
+  <si>
+    <t>OOSCO POSCO ENGINEERING &amp; CONSTRUCTION Co., LTD.
+2 Floor, My Dish Plaza, No.138 Tran Bind Str., Nam Tu Lies District, Hanoi, Vietnam
+E&amp;C Tel: 84-24-37957001 Fax: 84-24-37957005 Website: www,poscoenc.com
+Date : October 19, 2022
+Ref No.:  PSC-MLT-00446 -22-E
+To: Mr. Alain BECHEREAU - Project Director
+Systra Hanoi Metro Project Office
+Address: Level 12 -Hoa Bind Building, No. 106 Hoang Quot Viet, Can Gray District, Hanoi
+Tel: 84-24-3791 85 40 Fax: 84-24-37 91 85 44
+Ce: Mr. Nguyen Cao Mind — General Director
+Hanoi Metropolitan Railway Management Board (MRB)
+Address: CC2 Building, Dong Tau Urban Area, Hoang Mai, Hanoi
+Tel: 84-24-39 43 51 27 Tel: 84-24-39 43 51 26
+Subject: Co02— Notice on the readiness for acceptance of firefighting
+Reference:
+a. MRB’s letter Ref. No. 131/To-DSDT-HCTC on Notice on the conclusion of the General Director of
+MRB at the meeting on the implementation of acceptance and handover tasks of Line 3.1 dated
+28/09/2022.
+b. MRB’s letter Ref. 135/To-DSDT-HCTC on Notice on the conclusion of the General Director of MRB
+at the meeting on the implementation of acceptance and handover tasks of Line 3.] dated 6/10/2022
+c. PSC’s letter Ref, No. PSC-MLT-00112-22-E-V on Proposal for List of As-built drawings for FF
+inspection and acceptance dated 13/10/2022
+d. PIC’s letter PIC-MLT-03225-22-E-V on Relevant templates for Co's final acceptance for
+completion of the Firefighting System dated 14/10/2022.
+Dear Sir,
+Refer to the letter Ref [a], [b], [c], [đ] and the internal inspection result for completion of Fire fighting items
+between the Fire Fighting Consultant Unit (Thank Bind company - BCA) and PSC Contractor (Please see
+attachment #1 for the details). PSC Contractor would like to inform you that the works related to
+Firefighting acceptance have been prepared by the Contractor, and ready for PIC/MRB’s inspection before
+inviting the Fire Fighting Department for FF inspection of the Project. .
+PIC/MRB is kindly requested to soon notify the Contractor of inspection plan for completion of FF work
+under the package Co02.
+Your kind understanding and soon response would be highly appreciated.
+Attachment #1: Internal MOA for completion of Firefighting
+t1</t>
+  </si>
+  <si>
+    <t>Contract Package No 06: Notice of Claim under Clause 8.4 and 20.1 for delayed
+completion of earthing connection of false floor by CP02</t>
+  </si>
+  <si>
+    <t>Contract Package No 06: Warning to the Contractor's delays on the
+implementation of the Employer's requests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MU... UNINCORPORATED
+JOINT VENTURE
+ALSTOM -fi THALES
+Hanol, 06/08/2021
+To the attention of: Mr. Nguyen Cao Minh - General Director !
+, Hanoi Metropolitan Railway Management Board (MRB) |
+CC2 Building, Dong Tau Urban Area, Thinh Liet, Hoang Mai, Hanoi.
+Mr. Nguyen Ba Son - Manager of Project Implementation (PID1 Management)
+Hanoi Metropolitan Railway Management Board (MRB)
+PID1 Room, 3rd Floor, CC2 Building, Dong Tau Urban Area, Hoang Mai, Hanoi
+Copy to: Mr. Philippe BLANCHO - SYSTRA Project Director ‘ |
+Systra Hanoi Metro Project Office |
+412" floor — Hoa Binh Building,106 Hoang Quoc Viet Street, Cau Giay District, Hanoi
+Subject: Contract Package No 06: Warning to the Contractor's delays on the
+implementation of the Employer's requests (reply to 1303/DSDT-DA1)
+UJV Letter Reference No: UJV-MLT-00713-21-E-UJV
+Reference to Letter No / Date: [a] 1303/DSDT-DA1 dated 27/07/2021
+[b] UJV-MLT-00322-21-E-UJV dated 19/04/2021
+[c] UJV-MLT-00335-21-EV dated 23/04/2021
+[d] UJV-MLT-00435-21-EV dated 18/05/2021
+[e] UJV-MLT-00581-21-E-UJV dated 18/06/2021
+[f] UJV-MLT-00609-21-E-UJV dated 2/07/2021
+[g]1077/DSDT-DA1 received 29/06/2021
+[h] 868/DSDT-DA1 received 31/05/2021
+[i] 605/DSDT-DA1 received 28/04/2021
+[l] 446/DSDT-DA1 received 02/04/2021
+[k] UJV-MLT-00548-21-E-UJV dated 18/06/2021
+[m] UJV-MLT-00313-21-B-UJV dated 15/04/2021
+[n] UJV-MLT-00197-21-E-UJV dated 17/03/2021
+[I] UJV-MLT-00656-21-E-UJV dated 19/07/2021
+[o] UJV-MLT-00949-20-E-UJV dated 17/09/2020
+{p] UJV-MLT-00102-21-E-UJV dated 09/02/2021
+[q] UJV-MLT-01024-20-E dated 16/10/2020
+[r] UJV-MLT-00682-21-B dated 29/07/2021
+[s] UJV-MLT-01040-20-E dated 21/10/2020
+[t] PIC-MLT-03811-21-EV received 28/07/2021
+Dear Sirs,
+UJV acknowledges receipt of the above-captioned letter [a] from the Employer through email on 29 July 2021 and
+totally rejects the fully unfounded content of this letter. UJV Teminds that from the beginning of the project UJV has
+been very proactive and cooperative in order to move forward and speed-up the Hanoi L3 project in general and CP06
+in particular. On the specific matters raised by the Employer, UJV would like to respond item by item as follows.
+UJV refers to above-captioned letter {q] dated 16 October 2020, whereby we submitted draft Contract Amendment
+(including detailed 10 Annexes) for the operation of Elevated Section, and asked for discussion with the Employer the
+| UJV-MLT-00713-21-E-UJV dated:06/08/2021 Page 1 |
+ALSTOM Transport S.A. ~ HANOI LINE 3 / CP06 Project Office l .
+Suite 902, Capital Tower, 109 Tran Hung Dao Street, Cua Nam Ward, Hoan Kiem District, Hanoi, Vietnam
+Tel: + 84 (0)24 3956 4999 — Fax: +84 (0)24 3967 4999
 </t>
   </si>
 </sst>
@@ -1504,10 +2506,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D1131C8-FF00-D544-9C74-E364D352829E}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:B51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="168" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="168" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1716,6 +2718,214 @@
         <v>44</v>
       </c>
     </row>
+    <row r="26" spans="1:2" ht="245" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="301" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="242" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="249" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="308" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="267" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="188" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="201" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="231" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="252" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="271" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="240" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="231" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="283" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="298" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="246" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="279" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="277" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="330" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="A45" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="263" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="339" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="305" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="299" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="254" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="267" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>